<commit_message>
Update OASIS2 pipeline: fixed group coding, added longitudinal plots and metrics
</commit_message>
<xml_diff>
--- a/OASIS2_results/model_metrics.xlsx
+++ b/OASIS2_results/model_metrics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t xml:space="preserve">SVM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kNN</t>
   </si>
 </sst>
 </file>
@@ -374,7 +371,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.871635610766046</v>
+        <v>0.887</v>
       </c>
     </row>
     <row r="3">
@@ -382,7 +379,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.859213250517598</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4">
@@ -390,15 +387,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.853002070393375</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.544513457556936</v>
+        <v>0.656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>